<commit_message>
Add code for hw1 prb5 bme 6250
</commit_message>
<xml_diff>
--- a/BME6250-Biomech2/Homework1/data/hw1prb5_data.xlsx
+++ b/BME6250-Biomech2/Homework1/data/hw1prb5_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bulbasaur\GitHub\UtahCoursework\BME6250-Biomech2\Homework1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\GitHub\UtahCoursework\BME6250-Biomech2\Homework1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E01D0F9-B25F-475E-8556-758DCD9ACD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C16E72-76EF-4AB9-B1CC-CFD77918C1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="18600" windowHeight="13860" xr2:uid="{F436446C-328E-4481-B33E-D31FA4DFB03C}"/>
+    <workbookView xWindow="7590" yWindow="24285" windowWidth="21600" windowHeight="11385" xr2:uid="{F436446C-328E-4481-B33E-D31FA4DFB03C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>time</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>zInfStrain</t>
+  </si>
+  <si>
+    <t>xInfStrain</t>
+  </si>
+  <si>
+    <t>yStress</t>
+  </si>
+  <si>
+    <t>zStress</t>
+  </si>
+  <si>
+    <t>yDisplace</t>
+  </si>
+  <si>
+    <t>zDisplace</t>
   </si>
 </sst>
 </file>
@@ -90,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,15 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482CC456-02A3-425B-976A-EF24A98C06CB}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,16 +444,31 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -459,8 +490,23 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.02</v>
       </c>
@@ -474,16 +520,31 @@
         <v>0.01</v>
       </c>
       <c r="E3">
+        <v>-4.9262000000000004E-3</v>
+      </c>
+      <c r="F3">
+        <v>-4.9262000000000004E-3</v>
+      </c>
+      <c r="G3">
         <v>3.6477900000000001E-3</v>
       </c>
-      <c r="F3">
+      <c r="H3" s="1">
+        <v>3.3961200000000001E-6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3.3961200000000001E-6</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
         <v>-9.8524100000000007E-3</v>
       </c>
-      <c r="G3">
+      <c r="L3">
         <v>-9.8524100000000007E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.04</v>
       </c>
@@ -497,16 +558,31 @@
         <v>0.02</v>
       </c>
       <c r="E4">
+        <v>-9.7096000000000005E-3</v>
+      </c>
+      <c r="F4">
+        <v>-9.7096000000000005E-3</v>
+      </c>
+      <c r="G4">
         <v>7.6485099999999999E-3</v>
       </c>
-      <c r="F4">
+      <c r="H4" s="1">
+        <v>3.0756499999999999E-6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3.0756499999999999E-6</v>
+      </c>
+      <c r="J4">
+        <v>0.04</v>
+      </c>
+      <c r="K4">
         <v>-1.9419200000000001E-2</v>
       </c>
-      <c r="G4">
+      <c r="L4">
         <v>-1.9419200000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.06</v>
       </c>
@@ -520,16 +596,31 @@
         <v>0.03</v>
       </c>
       <c r="E5">
+        <v>-1.4357E-2</v>
+      </c>
+      <c r="F5">
+        <v>-1.4357E-2</v>
+      </c>
+      <c r="G5">
         <v>1.22232E-2</v>
       </c>
-      <c r="F5">
+      <c r="H5" s="1">
+        <v>2.7908E-6</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2.7908E-6</v>
+      </c>
+      <c r="J5">
+        <v>0.06</v>
+      </c>
+      <c r="K5">
         <v>-2.8713900000000001E-2</v>
       </c>
-      <c r="G5">
+      <c r="L5">
         <v>-2.8713900000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.08</v>
       </c>
@@ -543,16 +634,31 @@
         <v>0.04</v>
       </c>
       <c r="E6">
+        <v>-1.8874599999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>-1.8874599999999998E-2</v>
+      </c>
+      <c r="G6">
         <v>1.7602300000000001E-2</v>
       </c>
-      <c r="F6">
+      <c r="H6" s="1">
+        <v>2.5367000000000002E-6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.5367000000000002E-6</v>
+      </c>
+      <c r="J6">
+        <v>0.08</v>
+      </c>
+      <c r="K6">
         <v>-3.77493E-2</v>
       </c>
-      <c r="G6">
+      <c r="L6">
         <v>-3.77493E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.1</v>
       </c>
@@ -566,16 +672,31 @@
         <v>0.05</v>
       </c>
       <c r="E7">
+        <v>-2.3268500000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>-2.3268500000000001E-2</v>
+      </c>
+      <c r="G7">
         <v>2.40409E-2</v>
       </c>
-      <c r="F7">
+      <c r="H7" s="1">
+        <v>2.1744599999999998E-6</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.1744599999999998E-6</v>
+      </c>
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+      <c r="K7">
         <v>-4.6537000000000002E-2</v>
       </c>
-      <c r="G7">
+      <c r="L7">
         <v>-4.6537000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.12</v>
       </c>
@@ -589,16 +710,31 @@
         <v>0.06</v>
       </c>
       <c r="E8">
+        <v>-2.7544200000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>-2.7544200000000001E-2</v>
+      </c>
+      <c r="G8">
         <v>3.1830299999999999E-2</v>
       </c>
-      <c r="F8">
+      <c r="H8" s="1">
+        <v>5.6658900000000002E-7</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5.6658900000000002E-7</v>
+      </c>
+      <c r="J8">
+        <v>0.12</v>
+      </c>
+      <c r="K8">
         <v>-5.50883E-2</v>
       </c>
-      <c r="G8">
+      <c r="L8">
         <v>-5.50883E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.14000000000000001</v>
       </c>
@@ -612,16 +748,31 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E9">
+        <v>-3.17068E-2</v>
+      </c>
+      <c r="F9">
+        <v>-3.17068E-2</v>
+      </c>
+      <c r="G9">
         <v>4.1320500000000003E-2</v>
       </c>
-      <c r="F9">
+      <c r="H9" s="1">
+        <v>1.9226800000000001E-6</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1.9226800000000001E-6</v>
+      </c>
+      <c r="J9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K9">
         <v>-6.3413499999999998E-2</v>
       </c>
-      <c r="G9">
+      <c r="L9">
         <v>-6.3413600000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.16</v>
       </c>
@@ -635,16 +786,31 @@
         <v>0.08</v>
       </c>
       <c r="E10">
+        <v>-3.57612E-2</v>
+      </c>
+      <c r="F10">
+        <v>-3.57612E-2</v>
+      </c>
+      <c r="G10">
         <v>5.2919300000000002E-2</v>
       </c>
-      <c r="F10">
+      <c r="H10" s="1">
+        <v>-1.2777799999999999E-6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-1.2777799999999999E-6</v>
+      </c>
+      <c r="J10">
+        <v>0.16</v>
+      </c>
+      <c r="K10">
         <v>-7.1522500000000003E-2</v>
       </c>
-      <c r="G10">
+      <c r="L10">
         <v>-7.1522500000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.18</v>
       </c>
@@ -658,16 +824,31 @@
         <v>0.09</v>
       </c>
       <c r="E11">
+        <v>-3.9712200000000003E-2</v>
+      </c>
+      <c r="F11">
+        <v>-3.9712200000000003E-2</v>
+      </c>
+      <c r="G11">
         <v>6.7130999999999996E-2</v>
       </c>
-      <c r="F11">
+      <c r="H11" s="1">
+        <v>-4.6350599999999996E-6</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-4.6350599999999996E-6</v>
+      </c>
+      <c r="J11">
+        <v>0.18</v>
+      </c>
+      <c r="K11">
         <v>-7.9424400000000006E-2</v>
       </c>
-      <c r="G11">
+      <c r="L11">
         <v>-7.9424400000000006E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.2</v>
       </c>
@@ -681,16 +862,31 @@
         <v>0.1</v>
       </c>
       <c r="E12">
+        <v>-4.3563900000000003E-2</v>
+      </c>
+      <c r="F12">
+        <v>-4.3563900000000003E-2</v>
+      </c>
+      <c r="G12">
         <v>8.4576899999999997E-2</v>
       </c>
-      <c r="F12">
+      <c r="H12" s="1">
+        <v>-1.21816E-5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-1.21816E-5</v>
+      </c>
+      <c r="J12">
+        <v>0.2</v>
+      </c>
+      <c r="K12">
         <v>-8.7127800000000005E-2</v>
       </c>
-      <c r="G12">
+      <c r="L12">
         <v>-8.7127800000000005E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.22</v>
       </c>
@@ -704,16 +900,31 @@
         <v>0.11</v>
       </c>
       <c r="E13">
+        <v>-4.7320500000000001E-2</v>
+      </c>
+      <c r="F13">
+        <v>-4.7320500000000001E-2</v>
+      </c>
+      <c r="G13">
         <v>0.10602</v>
       </c>
-      <c r="F13">
+      <c r="H13" s="1">
+        <v>1.5890799999999999E-8</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1.5890799999999999E-8</v>
+      </c>
+      <c r="J13">
+        <v>0.22</v>
+      </c>
+      <c r="K13">
         <v>-9.46409E-2</v>
       </c>
-      <c r="G13">
+      <c r="L13">
         <v>-9.46409E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.24</v>
       </c>
@@ -727,16 +938,31 @@
         <v>0.12</v>
       </c>
       <c r="E14">
+        <v>-5.0985799999999998E-2</v>
+      </c>
+      <c r="F14">
+        <v>-5.0985799999999998E-2</v>
+      </c>
+      <c r="G14">
         <v>0.132415</v>
       </c>
-      <c r="F14">
+      <c r="H14" s="1">
+        <v>1.2556399999999999E-6</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1.2556399999999999E-6</v>
+      </c>
+      <c r="J14">
+        <v>0.24</v>
+      </c>
+      <c r="K14">
         <v>-0.10197199999999999</v>
       </c>
-      <c r="G14">
+      <c r="L14">
         <v>-0.10197199999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.26</v>
       </c>
@@ -750,16 +976,31 @@
         <v>0.13</v>
       </c>
       <c r="E15">
+        <v>-5.4563399999999998E-2</v>
+      </c>
+      <c r="F15">
+        <v>-5.4563399999999998E-2</v>
+      </c>
+      <c r="G15">
         <v>0.16494400000000001</v>
       </c>
-      <c r="F15">
+      <c r="H15" s="1">
+        <v>1.1575900000000001E-6</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1.1575900000000001E-6</v>
+      </c>
+      <c r="J15">
+        <v>0.26</v>
+      </c>
+      <c r="K15">
         <v>-0.109127</v>
       </c>
-      <c r="G15">
+      <c r="L15">
         <v>-0.109127</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.28000000000000003</v>
       </c>
@@ -773,16 +1014,31 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E16">
+        <v>-5.8056700000000003E-2</v>
+      </c>
+      <c r="F16">
+        <v>-5.8056700000000003E-2</v>
+      </c>
+      <c r="G16">
         <v>0.20515</v>
       </c>
-      <c r="F16">
+      <c r="H16" s="1">
+        <v>1.0684199999999999E-6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1.0684199999999999E-6</v>
+      </c>
+      <c r="J16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K16">
         <v>-0.11611299999999999</v>
       </c>
-      <c r="G16">
+      <c r="L16">
         <v>-0.11611299999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.3</v>
       </c>
@@ -796,16 +1052,31 @@
         <v>0.15</v>
       </c>
       <c r="E17">
+        <v>-6.1469099999999999E-2</v>
+      </c>
+      <c r="F17">
+        <v>-6.1469099999999999E-2</v>
+      </c>
+      <c r="G17">
         <v>0.254915</v>
       </c>
-      <c r="F17">
+      <c r="H17" s="1">
+        <v>9.862120000000001E-7</v>
+      </c>
+      <c r="I17" s="1">
+        <v>9.862120000000001E-7</v>
+      </c>
+      <c r="J17">
+        <v>0.3</v>
+      </c>
+      <c r="K17">
         <v>-0.12293800000000001</v>
       </c>
-      <c r="G17">
+      <c r="L17">
         <v>-0.12293800000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.32</v>
       </c>
@@ -819,16 +1090,31 @@
         <v>0.16</v>
       </c>
       <c r="E18">
+        <v>-6.4803600000000003E-2</v>
+      </c>
+      <c r="F18">
+        <v>-6.4803600000000003E-2</v>
+      </c>
+      <c r="G18">
         <v>0.31665500000000002</v>
       </c>
-      <c r="F18">
+      <c r="H18" s="1">
+        <v>9.0770000000000001E-7</v>
+      </c>
+      <c r="I18" s="1">
+        <v>9.0770000000000001E-7</v>
+      </c>
+      <c r="J18">
+        <v>0.32</v>
+      </c>
+      <c r="K18">
         <v>-0.129607</v>
       </c>
-      <c r="G18">
+      <c r="L18">
         <v>-0.129607</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.34</v>
       </c>
@@ -842,16 +1128,31 @@
         <v>0.17</v>
       </c>
       <c r="E19">
+        <v>-6.8062999999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>-6.8062999999999999E-2</v>
+      </c>
+      <c r="G19">
         <v>0.39344299999999999</v>
       </c>
-      <c r="F19">
+      <c r="H19" s="1">
+        <v>8.3090099999999998E-7</v>
+      </c>
+      <c r="I19" s="1">
+        <v>8.3090099999999998E-7</v>
+      </c>
+      <c r="J19">
+        <v>0.34</v>
+      </c>
+      <c r="K19">
         <v>-0.136126</v>
       </c>
-      <c r="G19">
+      <c r="L19">
         <v>-0.136126</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.36</v>
       </c>
@@ -865,16 +1166,31 @@
         <v>0.18</v>
       </c>
       <c r="E20">
+        <v>-7.1249999999999994E-2</v>
+      </c>
+      <c r="F20">
+        <v>-7.1249999999999994E-2</v>
+      </c>
+      <c r="G20">
         <v>0.48921100000000001</v>
       </c>
-      <c r="F20">
+      <c r="H20" s="1">
+        <v>7.6127700000000002E-7</v>
+      </c>
+      <c r="I20" s="1">
+        <v>7.6127700000000002E-7</v>
+      </c>
+      <c r="J20">
+        <v>0.36</v>
+      </c>
+      <c r="K20">
         <v>-0.14249999999999999</v>
       </c>
-      <c r="G20">
+      <c r="L20">
         <v>-0.14249999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.38</v>
       </c>
@@ -888,16 +1204,31 @@
         <v>0.19</v>
       </c>
       <c r="E21">
+        <v>-7.43674E-2</v>
+      </c>
+      <c r="F21">
+        <v>-7.43674E-2</v>
+      </c>
+      <c r="G21">
         <v>0.60902699999999999</v>
       </c>
-      <c r="F21">
+      <c r="H21" s="1">
+        <v>7.0755000000000001E-7</v>
+      </c>
+      <c r="I21" s="1">
+        <v>7.0755000000000001E-7</v>
+      </c>
+      <c r="J21">
+        <v>0.38</v>
+      </c>
+      <c r="K21">
         <v>-0.14873500000000001</v>
       </c>
-      <c r="G21">
+      <c r="L21">
         <v>-0.14873500000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.4</v>
       </c>
@@ -911,16 +1242,31 @@
         <v>0.2</v>
       </c>
       <c r="E22">
+        <v>-7.74175E-2</v>
+      </c>
+      <c r="F22">
+        <v>-7.74175E-2</v>
+      </c>
+      <c r="G22">
         <v>0.75936199999999998</v>
       </c>
-      <c r="F22">
+      <c r="H22" s="1">
+        <v>6.6709699999999995E-7</v>
+      </c>
+      <c r="I22" s="1">
+        <v>6.6709699999999995E-7</v>
+      </c>
+      <c r="J22">
+        <v>0.4</v>
+      </c>
+      <c r="K22">
         <v>-0.154835</v>
       </c>
-      <c r="G22">
+      <c r="L22">
         <v>-0.154835</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.42</v>
       </c>
@@ -934,16 +1280,31 @@
         <v>0.21</v>
       </c>
       <c r="E23">
+        <v>-8.0402699999999994E-2</v>
+      </c>
+      <c r="F23">
+        <v>-8.0402699999999994E-2</v>
+      </c>
+      <c r="G23">
         <v>0.94861399999999996</v>
       </c>
-      <c r="F23">
+      <c r="H23" s="1">
+        <v>6.2915000000000005E-7</v>
+      </c>
+      <c r="I23" s="1">
+        <v>6.2915000000000005E-7</v>
+      </c>
+      <c r="J23">
+        <v>0.42</v>
+      </c>
+      <c r="K23">
         <v>-0.160805</v>
       </c>
-      <c r="G23">
+      <c r="L23">
         <v>-0.160805</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.44</v>
       </c>
@@ -957,16 +1318,31 @@
         <v>0.22</v>
       </c>
       <c r="E24">
+        <v>-8.3325099999999999E-2</v>
+      </c>
+      <c r="F24">
+        <v>-8.3325099999999999E-2</v>
+      </c>
+      <c r="G24">
         <v>1.1876500000000001</v>
       </c>
-      <c r="F24">
+      <c r="H24" s="1">
+        <v>5.8973999999999999E-7</v>
+      </c>
+      <c r="I24" s="1">
+        <v>5.8973999999999999E-7</v>
+      </c>
+      <c r="J24">
+        <v>0.44</v>
+      </c>
+      <c r="K24">
         <v>-0.16664999999999999</v>
       </c>
-      <c r="G24">
+      <c r="L24">
         <v>-0.16664999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.46</v>
       </c>
@@ -980,16 +1356,31 @@
         <v>0.23</v>
       </c>
       <c r="E25">
+        <v>-8.6186799999999994E-2</v>
+      </c>
+      <c r="F25">
+        <v>-8.6186799999999994E-2</v>
+      </c>
+      <c r="G25">
         <v>1.4906200000000001</v>
       </c>
-      <c r="F25">
+      <c r="H25" s="1">
+        <v>5.5132700000000002E-7</v>
+      </c>
+      <c r="I25" s="1">
+        <v>5.5132700000000002E-7</v>
+      </c>
+      <c r="J25">
+        <v>0.46</v>
+      </c>
+      <c r="K25">
         <v>-0.172374</v>
       </c>
-      <c r="G25">
+      <c r="L25">
         <v>-0.172374</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.48</v>
       </c>
@@ -1003,16 +1394,31 @@
         <v>0.24</v>
       </c>
       <c r="E26">
+        <v>-8.8989700000000005E-2</v>
+      </c>
+      <c r="F26">
+        <v>-8.8989700000000005E-2</v>
+      </c>
+      <c r="G26">
         <v>1.8759699999999999</v>
       </c>
-      <c r="F26">
+      <c r="H26" s="1">
+        <v>5.15781E-7</v>
+      </c>
+      <c r="I26" s="1">
+        <v>5.15781E-7</v>
+      </c>
+      <c r="J26">
+        <v>0.48</v>
+      </c>
+      <c r="K26">
         <v>-0.177979</v>
       </c>
-      <c r="G26">
+      <c r="L26">
         <v>-0.177979</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.5</v>
       </c>
@@ -1026,16 +1432,31 @@
         <v>0.25</v>
       </c>
       <c r="E27">
+        <v>-9.17356E-2</v>
+      </c>
+      <c r="F27">
+        <v>-9.17356E-2</v>
+      </c>
+      <c r="G27">
         <v>2.3678400000000002</v>
       </c>
-      <c r="F27">
+      <c r="H27" s="1">
+        <v>4.8335100000000002E-7</v>
+      </c>
+      <c r="I27" s="1">
+        <v>4.8335100000000002E-7</v>
+      </c>
+      <c r="J27">
+        <v>0.5</v>
+      </c>
+      <c r="K27">
         <v>-0.183471</v>
       </c>
-      <c r="G27">
+      <c r="L27">
         <v>-0.183471</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.52</v>
       </c>
@@ -1049,16 +1470,31 @@
         <v>0.26</v>
       </c>
       <c r="E28">
+        <v>-9.4426200000000002E-2</v>
+      </c>
+      <c r="F28">
+        <v>-9.4426200000000002E-2</v>
+      </c>
+      <c r="G28">
         <v>2.99797</v>
       </c>
-      <c r="F28">
+      <c r="H28" s="1">
+        <v>4.5387700000000001E-7</v>
+      </c>
+      <c r="I28" s="1">
+        <v>4.5387700000000001E-7</v>
+      </c>
+      <c r="J28">
+        <v>0.52</v>
+      </c>
+      <c r="K28">
         <v>-0.18885199999999999</v>
       </c>
-      <c r="G28">
+      <c r="L28">
         <v>-0.18885199999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.54</v>
       </c>
@@ -1072,16 +1508,31 @@
         <v>0.27</v>
       </c>
       <c r="E29">
+        <v>-9.7062899999999994E-2</v>
+      </c>
+      <c r="F29">
+        <v>-9.7062899999999994E-2</v>
+      </c>
+      <c r="G29">
         <v>3.8081499999999999</v>
       </c>
-      <c r="F29">
+      <c r="H29" s="1">
+        <v>4.27186E-7</v>
+      </c>
+      <c r="I29" s="1">
+        <v>4.27186E-7</v>
+      </c>
+      <c r="J29">
+        <v>0.54</v>
+      </c>
+      <c r="K29">
         <v>-0.19412599999999999</v>
       </c>
-      <c r="G29">
+      <c r="L29">
         <v>-0.19412599999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.56000000000000005</v>
       </c>
@@ -1095,16 +1546,31 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E30">
+        <v>-9.9647200000000005E-2</v>
+      </c>
+      <c r="F30">
+        <v>-9.9647200000000005E-2</v>
+      </c>
+      <c r="G30">
         <v>4.8536599999999996</v>
       </c>
-      <c r="F30">
+      <c r="H30" s="1">
+        <v>4.0317399999999998E-7</v>
+      </c>
+      <c r="I30" s="1">
+        <v>4.0317399999999998E-7</v>
+      </c>
+      <c r="J30">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K30">
         <v>-0.199294</v>
       </c>
-      <c r="G30">
+      <c r="L30">
         <v>-0.199294</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.57999999999999996</v>
       </c>
@@ -1118,16 +1584,31 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E31">
+        <v>-0.10218000000000001</v>
+      </c>
+      <c r="F31">
+        <v>-0.10218000000000001</v>
+      </c>
+      <c r="G31">
         <v>6.2077600000000004</v>
       </c>
-      <c r="F31">
+      <c r="H31" s="1">
+        <v>3.8174799999999998E-7</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3.8174799999999998E-7</v>
+      </c>
+      <c r="J31">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K31">
         <v>-0.20436000000000001</v>
       </c>
-      <c r="G31">
+      <c r="L31">
         <v>-0.20436000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.6</v>
       </c>
@@ -1141,16 +1622,31 @@
         <v>0.3</v>
       </c>
       <c r="E32">
+        <v>-0.10466300000000001</v>
+      </c>
+      <c r="F32">
+        <v>-0.10466300000000001</v>
+      </c>
+      <c r="G32">
         <v>7.9678699999999996</v>
       </c>
-      <c r="F32">
+      <c r="H32" s="1">
+        <v>3.6285E-7</v>
+      </c>
+      <c r="I32" s="1">
+        <v>3.6285E-7</v>
+      </c>
+      <c r="J32">
+        <v>0.6</v>
+      </c>
+      <c r="K32">
         <v>-0.20932600000000001</v>
       </c>
-      <c r="G32">
+      <c r="L32">
         <v>-0.20932600000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.62</v>
       </c>
@@ -1164,16 +1660,31 @@
         <v>0.31</v>
       </c>
       <c r="E33">
+        <v>-0.107096</v>
+      </c>
+      <c r="F33">
+        <v>-0.107096</v>
+      </c>
+      <c r="G33">
         <v>10.2639</v>
       </c>
-      <c r="F33">
+      <c r="H33" s="1">
+        <v>3.46376E-7</v>
+      </c>
+      <c r="I33" s="1">
+        <v>3.46376E-7</v>
+      </c>
+      <c r="J33">
+        <v>0.62</v>
+      </c>
+      <c r="K33">
         <v>-0.21419099999999999</v>
       </c>
-      <c r="G33">
+      <c r="L33">
         <v>-0.21419099999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.64</v>
       </c>
@@ -1187,16 +1698,31 @@
         <v>0.32</v>
       </c>
       <c r="E34">
+        <v>-0.10947900000000001</v>
+      </c>
+      <c r="F34">
+        <v>-0.10947900000000001</v>
+      </c>
+      <c r="G34">
         <v>13.269299999999999</v>
       </c>
-      <c r="F34">
+      <c r="H34" s="1">
+        <v>3.32136E-7</v>
+      </c>
+      <c r="I34" s="1">
+        <v>3.32136E-7</v>
+      </c>
+      <c r="J34">
+        <v>0.64</v>
+      </c>
+      <c r="K34">
         <v>-0.21895800000000001</v>
       </c>
-      <c r="G34">
+      <c r="L34">
         <v>-0.21895800000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.66</v>
       </c>
@@ -1210,16 +1736,31 @@
         <v>0.33</v>
       </c>
       <c r="E35">
+        <v>-0.111813</v>
+      </c>
+      <c r="F35">
+        <v>-0.111813</v>
+      </c>
+      <c r="G35">
         <v>17.2166</v>
       </c>
-      <c r="F35">
+      <c r="H35" s="1">
+        <v>3.1959200000000002E-7</v>
+      </c>
+      <c r="I35" s="1">
+        <v>3.1959200000000002E-7</v>
+      </c>
+      <c r="J35">
+        <v>0.66</v>
+      </c>
+      <c r="K35">
         <v>-0.22362699999999999</v>
       </c>
-      <c r="G35">
+      <c r="L35">
         <v>-0.22362699999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.68</v>
       </c>
@@ -1233,16 +1774,31 @@
         <v>0.34</v>
       </c>
       <c r="E36">
+        <v>-0.114097</v>
+      </c>
+      <c r="F36">
+        <v>-0.114097</v>
+      </c>
+      <c r="G36">
         <v>22.417200000000001</v>
       </c>
-      <c r="F36">
+      <c r="H36" s="1">
+        <v>3.0746799999999998E-7</v>
+      </c>
+      <c r="I36" s="1">
+        <v>3.0746799999999998E-7</v>
+      </c>
+      <c r="J36">
+        <v>0.68</v>
+      </c>
+      <c r="K36">
         <v>-0.22819500000000001</v>
       </c>
-      <c r="G36">
+      <c r="L36">
         <v>-0.22819500000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.7</v>
       </c>
@@ -1256,16 +1812,31 @@
         <v>0.35</v>
       </c>
       <c r="E37">
+        <v>-0.11633</v>
+      </c>
+      <c r="F37">
+        <v>-0.11633</v>
+      </c>
+      <c r="G37">
         <v>29.288799999999998</v>
       </c>
-      <c r="F37">
+      <c r="H37" s="1">
+        <v>2.9264800000000001E-7</v>
+      </c>
+      <c r="I37" s="1">
+        <v>2.9264800000000001E-7</v>
+      </c>
+      <c r="J37">
+        <v>0.7</v>
+      </c>
+      <c r="K37">
         <v>-0.23266000000000001</v>
       </c>
-      <c r="G37">
+      <c r="L37">
         <v>-0.23266000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.72</v>
       </c>
@@ -1279,16 +1850,31 @@
         <v>0.36</v>
       </c>
       <c r="E38">
+        <v>-0.118509</v>
+      </c>
+      <c r="F38">
+        <v>-0.118509</v>
+      </c>
+      <c r="G38">
         <v>38.391500000000001</v>
       </c>
-      <c r="F38">
+      <c r="H38" s="1">
+        <v>2.6777200000000002E-7</v>
+      </c>
+      <c r="I38" s="1">
+        <v>2.6777200000000002E-7</v>
+      </c>
+      <c r="J38">
+        <v>0.72</v>
+      </c>
+      <c r="K38">
         <v>-0.23701800000000001</v>
       </c>
-      <c r="G38">
+      <c r="L38">
         <v>-0.23701800000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.74</v>
       </c>
@@ -1302,16 +1888,31 @@
         <v>0.37</v>
       </c>
       <c r="E39">
+        <v>-0.120631</v>
+      </c>
+      <c r="F39">
+        <v>-0.120631</v>
+      </c>
+      <c r="G39">
         <v>50.474400000000003</v>
       </c>
-      <c r="F39">
+      <c r="H39" s="1">
+        <v>2.1538399999999999E-7</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2.1538399999999999E-7</v>
+      </c>
+      <c r="J39">
+        <v>0.74</v>
+      </c>
+      <c r="K39">
         <v>-0.24126300000000001</v>
       </c>
-      <c r="G39">
+      <c r="L39">
         <v>-0.24126300000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.76</v>
       </c>
@@ -1325,16 +1926,31 @@
         <v>0.38</v>
       </c>
       <c r="E40">
+        <v>-0.122692</v>
+      </c>
+      <c r="F40">
+        <v>-0.122692</v>
+      </c>
+      <c r="G40">
         <v>66.535200000000003</v>
       </c>
-      <c r="F40">
+      <c r="H40" s="1">
+        <v>9.3607100000000004E-8</v>
+      </c>
+      <c r="I40" s="1">
+        <v>9.3607100000000004E-8</v>
+      </c>
+      <c r="J40">
+        <v>0.76</v>
+      </c>
+      <c r="K40">
         <v>-0.24538299999999999</v>
       </c>
-      <c r="G40">
+      <c r="L40">
         <v>-0.24538299999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.78</v>
       </c>
@@ -1348,16 +1964,31 @@
         <v>0.39</v>
       </c>
       <c r="E41">
+        <v>-0.124683</v>
+      </c>
+      <c r="F41">
+        <v>-0.124683</v>
+      </c>
+      <c r="G41">
         <v>87.894000000000005</v>
       </c>
-      <c r="F41">
+      <c r="H41" s="1">
+        <v>-1.9983399999999999E-7</v>
+      </c>
+      <c r="I41" s="1">
+        <v>-1.9983399999999999E-7</v>
+      </c>
+      <c r="J41">
+        <v>0.78</v>
+      </c>
+      <c r="K41">
         <v>-0.249366</v>
       </c>
-      <c r="G41">
+      <c r="L41">
         <v>-0.249366</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.8</v>
       </c>
@@ -1371,16 +2002,31 @@
         <v>0.4</v>
       </c>
       <c r="E42">
+        <v>-0.12659599999999999</v>
+      </c>
+      <c r="F42">
+        <v>-0.12659599999999999</v>
+      </c>
+      <c r="G42">
         <v>116.27800000000001</v>
       </c>
-      <c r="F42">
+      <c r="H42" s="1">
+        <v>-9.1968000000000004E-7</v>
+      </c>
+      <c r="I42" s="1">
+        <v>-9.1968000000000004E-7</v>
+      </c>
+      <c r="J42">
+        <v>0.8</v>
+      </c>
+      <c r="K42">
         <v>-0.25319199999999997</v>
       </c>
-      <c r="G42">
+      <c r="L42">
         <v>-0.25319199999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.82</v>
       </c>
@@ -1394,16 +2040,31 @@
         <v>0.41</v>
       </c>
       <c r="E43">
+        <v>-0.128418</v>
+      </c>
+      <c r="F43">
+        <v>-0.128418</v>
+      </c>
+      <c r="G43">
         <v>153.911</v>
       </c>
-      <c r="F43">
+      <c r="H43" s="1">
+        <v>-2.7114399999999998E-6</v>
+      </c>
+      <c r="I43" s="1">
+        <v>-2.7114399999999998E-6</v>
+      </c>
+      <c r="J43">
+        <v>0.82</v>
+      </c>
+      <c r="K43">
         <v>-0.25683699999999998</v>
       </c>
-      <c r="G43">
+      <c r="L43">
         <v>-0.25683699999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.84</v>
       </c>
@@ -1417,16 +2078,31 @@
         <v>0.42</v>
       </c>
       <c r="E44">
+        <v>-0.130134</v>
+      </c>
+      <c r="F44">
+        <v>-0.130134</v>
+      </c>
+      <c r="G44">
         <v>203.59</v>
       </c>
-      <c r="F44">
+      <c r="H44" s="1">
+        <v>-7.2282399999999999E-6</v>
+      </c>
+      <c r="I44" s="1">
+        <v>-7.2282399999999999E-6</v>
+      </c>
+      <c r="J44">
+        <v>0.84</v>
+      </c>
+      <c r="K44">
         <v>-0.26026700000000003</v>
       </c>
-      <c r="G44">
+      <c r="L44">
         <v>-0.26026700000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.86</v>
       </c>
@@ -1440,16 +2116,31 @@
         <v>0.43</v>
       </c>
       <c r="E45">
+        <v>-0.13172200000000001</v>
+      </c>
+      <c r="F45">
+        <v>-0.13172200000000001</v>
+      </c>
+      <c r="G45">
         <v>268.72199999999998</v>
       </c>
-      <c r="F45">
+      <c r="H45" s="1">
+        <v>-1.87012E-5</v>
+      </c>
+      <c r="I45" s="1">
+        <v>-1.87012E-5</v>
+      </c>
+      <c r="J45">
+        <v>0.86</v>
+      </c>
+      <c r="K45">
         <v>-0.26344299999999998</v>
       </c>
-      <c r="G45">
+      <c r="L45">
         <v>-0.26344299999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.88</v>
       </c>
@@ -1463,16 +2154,31 @@
         <v>0.44</v>
       </c>
       <c r="E46">
+        <v>-0.133158</v>
+      </c>
+      <c r="F46">
+        <v>-0.133158</v>
+      </c>
+      <c r="G46">
         <v>353.267</v>
       </c>
-      <c r="F46">
+      <c r="H46" s="1">
+        <v>-4.7790300000000002E-5</v>
+      </c>
+      <c r="I46" s="1">
+        <v>-4.7790300000000002E-5</v>
+      </c>
+      <c r="J46">
+        <v>0.88</v>
+      </c>
+      <c r="K46">
         <v>-0.266316</v>
       </c>
-      <c r="G46">
+      <c r="L46">
         <v>-0.266316</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.9</v>
       </c>
@@ -1486,16 +2192,31 @@
         <v>0.45</v>
       </c>
       <c r="E47">
+        <v>-0.13441600000000001</v>
+      </c>
+      <c r="F47">
+        <v>-0.13441600000000001</v>
+      </c>
+      <c r="G47">
         <v>461.54599999999999</v>
       </c>
-      <c r="F47">
+      <c r="H47" s="1">
+        <v>-2.4906799999999999E-9</v>
+      </c>
+      <c r="I47" s="1">
+        <v>-2.49067E-9</v>
+      </c>
+      <c r="J47">
+        <v>0.9</v>
+      </c>
+      <c r="K47">
         <v>-0.26883299999999999</v>
       </c>
-      <c r="G47">
+      <c r="L47">
         <v>-0.26883299999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.92</v>
       </c>
@@ -1509,16 +2230,31 @@
         <v>0.46</v>
       </c>
       <c r="E48">
+        <v>-0.13546800000000001</v>
+      </c>
+      <c r="F48">
+        <v>-0.13546800000000001</v>
+      </c>
+      <c r="G48">
         <v>597.86800000000005</v>
       </c>
-      <c r="F48">
+      <c r="H48" s="1">
+        <v>-1.26155E-8</v>
+      </c>
+      <c r="I48" s="1">
+        <v>-1.26155E-8</v>
+      </c>
+      <c r="J48">
+        <v>0.92</v>
+      </c>
+      <c r="K48">
         <v>-0.27093600000000001</v>
       </c>
-      <c r="G48">
+      <c r="L48">
         <v>-0.27093600000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.94</v>
       </c>
@@ -1532,16 +2268,31 @@
         <v>0.47</v>
       </c>
       <c r="E49">
+        <v>-0.13628499999999999</v>
+      </c>
+      <c r="F49">
+        <v>-0.13628499999999999</v>
+      </c>
+      <c r="G49">
         <v>765.99300000000005</v>
       </c>
-      <c r="F49">
+      <c r="H49" s="1">
+        <v>-6.1605399999999997E-8</v>
+      </c>
+      <c r="I49" s="1">
+        <v>-6.1605399999999997E-8</v>
+      </c>
+      <c r="J49">
+        <v>0.94</v>
+      </c>
+      <c r="K49">
         <v>-0.27257100000000001</v>
       </c>
-      <c r="G49">
+      <c r="L49">
         <v>-0.27257100000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.96</v>
       </c>
@@ -1555,16 +2306,31 @@
         <v>0.48</v>
       </c>
       <c r="E50">
+        <v>-0.136846</v>
+      </c>
+      <c r="F50">
+        <v>-0.136846</v>
+      </c>
+      <c r="G50">
         <v>968.52599999999995</v>
       </c>
-      <c r="F50">
+      <c r="H50" s="1">
+        <v>-2.9416100000000001E-7</v>
+      </c>
+      <c r="I50" s="1">
+        <v>-2.9416100000000001E-7</v>
+      </c>
+      <c r="J50">
+        <v>0.96</v>
+      </c>
+      <c r="K50">
         <v>-0.27369300000000002</v>
       </c>
-      <c r="G50">
+      <c r="L50">
         <v>-0.27369300000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.98</v>
       </c>
@@ -1578,16 +2344,31 @@
         <v>0.49</v>
       </c>
       <c r="E51">
+        <v>-0.13713600000000001</v>
+      </c>
+      <c r="F51">
+        <v>-0.13713600000000001</v>
+      </c>
+      <c r="G51">
         <v>1206.4000000000001</v>
       </c>
-      <c r="F51">
+      <c r="H51" s="1">
+        <v>-1.4828E-6</v>
+      </c>
+      <c r="I51" s="1">
+        <v>-1.4828E-6</v>
+      </c>
+      <c r="J51">
+        <v>0.98</v>
+      </c>
+      <c r="K51">
         <v>-0.27427200000000002</v>
       </c>
-      <c r="G51">
+      <c r="L51">
         <v>-0.27427200000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1601,12 +2382,27 @@
         <v>0.5</v>
       </c>
       <c r="E52">
+        <v>-0.13714899999999999</v>
+      </c>
+      <c r="F52">
+        <v>-0.13714899999999999</v>
+      </c>
+      <c r="G52">
         <v>1478.64</v>
       </c>
-      <c r="F52">
+      <c r="H52" s="1">
+        <v>-4.24194E-12</v>
+      </c>
+      <c r="I52" s="1">
+        <v>-4.2703600000000004E-12</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
         <v>-0.27429799999999999</v>
       </c>
-      <c r="G52">
+      <c r="L52">
         <v>-0.27429799999999999</v>
       </c>
     </row>

</xml_diff>